<commit_message>
إضافة حدث جديد في Card21 by admin at 2025-12-10 12:59:51
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -7435,66 +7435,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7527,51 +7479,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7589,66 +7509,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7666,11 +7538,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7686,46 +7554,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>28\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7748,61 +7592,25 @@
           <t>578</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>13\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7825,36 +7633,16 @@
           <t>749</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7865,21 +7653,9 @@
           <t>19\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7902,11 +7678,7 @@
           <t>880</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7917,46 +7689,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>5\10\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7984,51 +7728,19 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>26/11/2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t>م محمد عبدالله ،ف.محمود ايهاب</t>
@@ -8051,66 +7763,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8128,66 +7792,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8205,66 +7821,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8272,56 +7840,16 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
           <t>20/9/2025</t>
@@ -8349,56 +7877,16 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>21\7\2025</t>
@@ -8426,66 +7914,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>14\8\2024</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>تم تشحيم المكنه + عمل صيانه</t>
@@ -8503,66 +7947,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>25\8\2024</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>تم عمل معايره للمكنه setting</t>
@@ -8580,66 +7980,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
           <t>14\10\2024</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
           <t>تم عمل صيانه نصف سنويه</t>
@@ -8657,66 +8013,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
           <t>14\10\2024</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>تم تغيير السستم من ax الي ay</t>
@@ -8734,66 +8046,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
           <t>31\12\2025</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>تم عمل صيانه نصف سنويه</t>
@@ -8811,66 +8079,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
           <t>9\1\2025</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>تم عمل معايره وصيانه نصف سنويه</t>
@@ -8888,56 +8112,16 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
           <t>23/11/2025</t>
@@ -8965,66 +8149,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
           <t>18\1\2025</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
           <t>تم سن الفلاتس والسليندر ومعايره المكنه وتغيير الجرائد الخلفيه (1_5_8)</t>
@@ -9042,66 +8182,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
           <t>13\4\2025</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
           <t>تم تغيير الجرائد الاماميه(1_2_4_5_7_8)</t>
@@ -9119,66 +8215,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
           <t>24\4\2025</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr">
         <is>
           <t>تم تغيير شداد السليندر والليكران والشداد العلوي</t>
@@ -9196,66 +8248,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
           <t>10\7\2025</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
           <t>تم تغيير زيت الجيربوكس</t>
@@ -9273,66 +8281,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
           <t>19\7\2025</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr">
         <is>
           <t>تم تغيير الفلاتس وجريده 1</t>
@@ -9350,66 +8314,22 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
           <t>19\7\2025</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
           <t>تم تغير الجرائد الخلفيه (1_5_8)</t>
@@ -9427,56 +8347,16 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
           <t>26\11\2025</t>
@@ -9504,56 +8384,16 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
           <t>9/12/2025</t>
@@ -17688,7 +16528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17789,18 +16629,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -17818,18 +16706,66 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -17847,18 +16783,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -17876,7 +16860,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -17892,18 +16880,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>21\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -17926,25 +16942,61 @@
           <t>610</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>13\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -17967,7 +17019,11 @@
           <t>796</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -17978,18 +17034,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>31\8\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -18007,18 +17091,66 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -18036,18 +17168,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -18065,18 +17245,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -18094,18 +17322,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -18123,18 +17399,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -18142,22 +17466,66 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>10\8\2024</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr">
         <is>
           <t>تم تشحيم المكنه بالكامل +عمل صيانه</t>
@@ -18175,22 +17543,66 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>28\8\2024</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N14" t="inlineStr">
         <is>
           <t>تم عمل معايره للمكنه steeing</t>
@@ -18208,22 +17620,66 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>28\8\2024</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>تم عمل معايره للمكنه setting</t>
@@ -18241,22 +17697,66 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>6\11\2024</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr">
         <is>
           <t>تم عمل مرجعه علي معيار المكنه بسبب مشكله في cv</t>
@@ -18274,16 +17774,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>19\12\2024</t>
@@ -18311,22 +17851,66 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>21\1\2025</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr">
         <is>
           <t>تم سن الفلاتس والسليندر وتغيير الجرائد الخلفيه ومعياره المكنه (1_5_8)</t>
@@ -18344,16 +17928,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
           <t>13\5\2025</t>
@@ -18381,16 +18005,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>14\8\2025</t>
@@ -18418,16 +18082,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>31\8\2025</t>
@@ -18455,16 +18159,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
           <t>11/2/2025</t>
@@ -18492,16 +18236,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>4/5/2025</t>
@@ -18529,16 +18313,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
           <t>29/6/2025</t>
@@ -18566,16 +18390,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
           <t>20/9/2025</t>
@@ -18603,16 +18467,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
           <t>11/2/2025</t>
@@ -18640,16 +18544,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
           <t>19/10/2025</t>
@@ -18677,16 +18621,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>9/12/2025</t>
@@ -18705,6 +18689,47 @@
       <c r="O28" t="inlineStr">
         <is>
           <t>مصطفى</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>سيرفيس</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>تم تغيير الفلاتس المتحركة 
+وتم سن السلندر6شوط
+وتم سن الدوفر 2شوط
+وتم تغيير اول جريده 240
+ملحوظه (حاله السلندر سئه)</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>م .محمد عبدالله ،تيم الكرد</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:06:55
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17093,7 +17093,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>966.5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -18698,16 +18698,56 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
           <t>10/12/2025</t>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:08:21
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17039,11 +17039,7 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>✅</t>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:08:31
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17039,7 +17039,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
           <t>✅</t>
@@ -17114,7 +17118,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:08:42
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17044,11 +17044,7 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✅</t>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:08:55
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17044,7 +17044,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✅</t>
@@ -17119,7 +17123,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:09:07
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17049,11 +17049,7 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>31\8\2025</t>

</xml_diff>

<commit_message>
تعديل تلقائي في شيت Card21 by admin at 2025-12-10 13:09:18
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -17049,7 +17049,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>31\8\2025</t>
@@ -17124,7 +17128,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">

</xml_diff>

<commit_message>
إضافة حدث جديد في Card13 by admin at 2025-12-11 08:45:05
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -3111,7 +3111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3212,18 +3212,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3256,19 +3304,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>24\12\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3286,18 +3366,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3315,8 +3443,16 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3327,18 +3463,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>9\3\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3361,25 +3525,61 @@
           <t>576</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3402,16 +3602,36 @@
           <t>758</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3422,9 +3642,21 @@
           <t>24\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3442,22 +3674,46 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>2/12/2025</t>
@@ -3500,7 +3756,11 @@
           <t>875</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3511,18 +3771,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>15\10\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3540,18 +3828,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3569,18 +3905,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3598,18 +3982,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3627,18 +4059,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3646,16 +4126,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>13\8\2024</t>
@@ -3666,7 +4186,11 @@
           <t>تم تشحيم المكنه الكامل +عمل صيانه</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O14" t="inlineStr">
         <is>
           <t>تيم العمل</t>
@@ -3679,16 +4203,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>14\12\2024</t>
@@ -3699,7 +4263,11 @@
           <t>تم عمل صيانه نصف سنويه</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O15" t="inlineStr">
         <is>
           <t>تيم العمل</t>
@@ -3712,16 +4280,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>24\12\2024</t>
@@ -3732,7 +4340,11 @@
           <t>تم سن الفلاتس ومعايره</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O16" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -3745,16 +4357,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>20\4\2025</t>
@@ -3782,16 +4434,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>12\8\2025</t>
@@ -3819,16 +4511,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
           <t>9\3\2025</t>
@@ -3839,7 +4571,11 @@
           <t>تم تغيير الجرائد الخلفيه ومعايرته</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -3852,16 +4588,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>24\7\2025</t>
@@ -3872,7 +4648,11 @@
           <t>تم تغيير الفلاتس وتغيير جريد 1</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O20" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -3885,16 +4665,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>24/3/2025</t>
@@ -3922,16 +4742,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
           <t>15\10\2025</t>
@@ -3942,7 +4802,11 @@
           <t>تم تغيير الجرائد الخلفيه (1_5_8)</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O22" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -3955,16 +4819,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>2\12\2025</t>
@@ -3975,7 +4879,11 @@
           <t>تم سن السليندر والفلاتس (10 شوط)</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O23" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -3988,16 +4896,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
           <t>5/10/2025</t>
@@ -4025,16 +4973,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
           <t>17/11/2025</t>
@@ -4062,16 +5050,56 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
           <t>17/11/2025</t>
@@ -4090,6 +5118,43 @@
       <c r="O26" t="inlineStr">
         <is>
           <t>فني</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>تم تغير المفتاح بمحلي</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>انكسار مفتاح سيرفيس بالماكينه  وعطل مفتاح</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>م.محمود امين</t>
         </is>
       </c>
     </row>
@@ -16528,7 +17593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16629,66 +17694,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -16706,66 +17723,18 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -16783,66 +17752,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -16860,11 +17781,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -16880,46 +17797,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>21\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -16942,61 +17831,25 @@
           <t>610</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>13\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -17019,11 +17872,7 @@
           <t>796</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -17034,46 +17883,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>31\8\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -17091,66 +17912,18 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>966.5</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>10/12/2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله ،تيم الكرد</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -17168,66 +17941,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -17245,66 +17970,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -17322,66 +17999,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -17399,66 +18028,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -17466,66 +18047,22 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
           <t>10\8\2024</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
           <t>تم تشحيم المكنه بالكامل +عمل صيانه</t>
@@ -17543,66 +18080,22 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>28\8\2024</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
           <t>تم عمل معايره للمكنه steeing</t>
@@ -17620,66 +18113,22 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>28\8\2024</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>تم عمل معايره للمكنه setting</t>
@@ -17697,66 +18146,22 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>6\11\2024</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>تم عمل مرجعه علي معيار المكنه بسبب مشكله في cv</t>
@@ -17774,56 +18179,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
           <t>19\12\2024</t>
@@ -17851,66 +18216,22 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
           <t>21\1\2025</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>تم سن الفلاتس والسليندر وتغيير الجرائد الخلفيه ومعياره المكنه (1_5_8)</t>
@@ -17928,56 +18249,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
           <t>13\5\2025</t>
@@ -18005,56 +18286,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
           <t>14\8\2025</t>
@@ -18082,56 +18323,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
           <t>31\8\2025</t>
@@ -18159,56 +18360,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
           <t>11/2/2025</t>
@@ -18236,56 +18397,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
           <t>4/5/2025</t>
@@ -18313,56 +18434,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
           <t>29/6/2025</t>
@@ -18390,56 +18471,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
           <t>20/9/2025</t>
@@ -18467,56 +18508,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
           <t>11/2/2025</t>
@@ -18544,56 +18545,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
           <t>19/10/2025</t>
@@ -18621,56 +18582,16 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
           <t>9/12/2025</t>
@@ -18689,87 +18610,6 @@
       <c r="O28" t="inlineStr">
         <is>
           <t>مصطفى</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>10/12/2025</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>سيرفيس</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>تم تغيير الفلاتس المتحركة 
-وتم سن السلندر6شوط
-وتم سن الدوفر 2شوط
-وتم تغيير اول جريده 240
-ملحوظه (حاله السلندر سئه)</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>م .محمد عبدالله ،تيم الكرد</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-11 08:54:31
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -3212,66 +3212,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3304,51 +3256,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>24\12\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3366,66 +3286,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3443,16 +3315,8 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3463,46 +3327,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>9\3\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3525,61 +3361,25 @@
           <t>576</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3602,36 +3402,16 @@
           <t>758</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3642,21 +3422,9 @@
           <t>24\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3674,46 +3442,22 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>2/12/2025</t>
@@ -3756,11 +3500,7 @@
           <t>875</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -3771,46 +3511,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>15\10\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3828,66 +3540,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3905,66 +3569,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3982,66 +3598,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4059,66 +3627,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4126,56 +3646,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>13\8\2024</t>
@@ -4186,11 +3666,7 @@
           <t>تم تشحيم المكنه الكامل +عمل صيانه</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>تيم العمل</t>
@@ -4203,56 +3679,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>14\12\2024</t>
@@ -4263,11 +3699,7 @@
           <t>تم عمل صيانه نصف سنويه</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>تيم العمل</t>
@@ -4280,56 +3712,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>24\12\2024</t>
@@ -4340,11 +3732,7 @@
           <t>تم سن الفلاتس ومعايره</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -4357,56 +3745,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
           <t>20\4\2025</t>
@@ -4434,56 +3782,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
           <t>12\8\2025</t>
@@ -4511,56 +3819,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
           <t>9\3\2025</t>
@@ -4571,11 +3839,7 @@
           <t>تم تغيير الجرائد الخلفيه ومعايرته</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -4588,56 +3852,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
           <t>24\7\2025</t>
@@ -4648,11 +3872,7 @@
           <t>تم تغيير الفلاتس وتغيير جريد 1</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -4665,56 +3885,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
           <t>24/3/2025</t>
@@ -4742,56 +3922,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
           <t>15\10\2025</t>
@@ -4802,11 +3942,7 @@
           <t>تم تغيير الجرائد الخلفيه (1_5_8)</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -4819,56 +3955,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
           <t>2\12\2025</t>
@@ -4879,11 +3975,7 @@
           <t>تم سن السليندر والفلاتس (10 شوط)</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
           <t>الخبير</t>
@@ -4896,56 +3988,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
           <t>5/10/2025</t>
@@ -4973,56 +4025,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
           <t>17/11/2025</t>
@@ -5050,56 +4062,16 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
           <t>17/11/2025</t>
@@ -15839,7 +14811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15940,21 +14912,61 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم الشتغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>A.Elshenawy</t>
@@ -15977,7 +14989,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -15988,19 +15004,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -16018,7 +15066,11 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -16034,18 +15086,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -16063,18 +15143,66 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -16097,25 +15225,61 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -16138,16 +15302,36 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -16158,9 +15342,21 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -16183,7 +15379,11 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -16194,17 +15394,41 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -16237,12 +15461,36 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -16253,7 +15501,11 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -16276,18 +15528,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -16305,18 +15605,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -16334,18 +15682,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -16363,18 +15759,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -16382,16 +15826,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>30/6/2025</t>
@@ -16419,16 +15903,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>22/10/2025</t>
@@ -16456,16 +15980,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>11/11/2025</t>
@@ -16493,16 +16057,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>15/11/2025</t>
@@ -16521,6 +16125,43 @@
       <c r="O17" t="inlineStr">
         <is>
           <t>فني</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>وجود صوت عالي في منطقه الدلڤري الامامي</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>تم تغير 2بليه 6006   في اكس الدلڤري الامامي</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>م/محمد عبدالله/ايهاب</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-11 08:56:55
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -14811,7 +14811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16134,16 +16134,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>11/12/2025</t>
@@ -16160,6 +16200,43 @@
         </is>
       </c>
       <c r="O18" t="inlineStr">
+        <is>
+          <t>م/محمد عبدالله/ايهاب</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>قطع سير 700</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>تم تغير سير مشرشر  700مجموعه الكلندرات</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>م/محمد عبدالله/ايهاب</t>
         </is>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card23 by admin at 2025-12-11 11:16:48
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -10422,7 +10422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10523,18 +10523,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10552,7 +10600,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10563,19 +10615,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10593,18 +10677,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10622,7 +10754,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10638,22 +10774,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10676,25 +10836,61 @@
           <t>641</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10717,7 +10913,11 @@
           <t>836</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10728,18 +10928,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10762,14 +10990,26 @@
           <t>995</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>✅</t>
@@ -10790,7 +11030,11 @@
           <t>6/12/2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr">
         <is>
           <t>تم تغير فلاتس متحركه واول جريده240 وسن دوفر 2شوط وسلندر6شوط</t>
@@ -10818,18 +11062,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10847,18 +11139,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10876,18 +11216,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10905,18 +11293,66 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10924,22 +11360,66 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr">
         <is>
           <t>تم سن الفلاتس وتغيير اول جريده فوق المنشار</t>
@@ -10957,16 +11437,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>10\8\2024</t>
@@ -10994,22 +11514,66 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>تم عمل setting كامل للمكنه وتضيق المسافات</t>
@@ -11027,16 +11591,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>18\12\2024</t>
@@ -11064,22 +11668,66 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr">
         <is>
           <t>تم سن الفلاتس والسلندر وتغيير الجرائد ومعايره</t>
@@ -11097,16 +11745,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>15\5\2025</t>
@@ -11134,16 +11822,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
           <t>14\8\2025</t>
@@ -11171,16 +11899,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>4\9\2025</t>
@@ -11208,16 +11976,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>6\12\2025</t>
@@ -11245,16 +12053,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
           <t>15/11/2025</t>
@@ -11282,16 +12130,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>15/11/2025</t>
@@ -11319,16 +12207,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
           <t>22/2/2025</t>
@@ -11347,6 +12275,46 @@
       <c r="O24" t="inlineStr">
         <is>
           <t>فني</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>نبس عالي</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>تم تغير جريده الليكر أن العلويه T.S90
+وتم أعاده عيار ماكينه بالكامل 
+جرائد خلفيه. 18.16.14ساو بالترتيب 
+و جرائد اماميه 12ساو</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله،تيم الكرد</t>
         </is>
       </c>
     </row>
@@ -14912,61 +15880,21 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم الشتغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>A.Elshenawy</t>
@@ -14989,11 +15917,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -15004,51 +15928,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -15066,11 +15958,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -15086,46 +15974,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -15143,66 +16003,18 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -15225,61 +16037,25 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -15302,36 +16078,16 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -15342,21 +16098,9 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -15379,11 +16123,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -15394,41 +16134,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -15461,36 +16177,12 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -15501,11 +16193,7 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -15528,66 +16216,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -15605,66 +16245,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -15682,66 +16274,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -15759,66 +16303,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -15826,56 +16322,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>30/6/2025</t>
@@ -15903,56 +16359,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>22/10/2025</t>
@@ -15980,56 +16396,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>11/11/2025</t>
@@ -16057,56 +16433,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
           <t>15/11/2025</t>
@@ -16134,56 +16470,16 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
           <t>11/12/2025</t>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card24 by admin at 2026-02-01 20:11:00
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2824,26 +2824,113 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr">
         <is>
           <t>خلل</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>خلل</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة عمود جديد 'correction' إلى شيت 'سحب1' by admin at 2026-02-01 20:30:38
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -18093,7 +18093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18140,6 +18140,11 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>event</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>correction</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة عمود جديد 'servised by' إلى شيت 'سحب1' by admin at 2026-02-01 20:31:04
</commit_message>
<xml_diff>
--- a/l4.xlsx
+++ b/l4.xlsx
@@ -18093,7 +18093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18145,6 +18145,11 @@
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>correction</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>servised by</t>
         </is>
       </c>
     </row>

</xml_diff>